<commit_message>
intellij shortcuts page formatting
</commit_message>
<xml_diff>
--- a/IntelliJ-Shortcuts.xlsx
+++ b/IntelliJ-Shortcuts.xlsx
@@ -1356,7 +1356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A25" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2343,7 +2343,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.19685039370078741" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="72" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"-,Fett"&amp;14IntelliJ Shortcuts</oddHeader>

</xml_diff>

<commit_message>
intellij shortcuts - simplify markups
</commit_message>
<xml_diff>
--- a/IntelliJ-Shortcuts.xlsx
+++ b/IntelliJ-Shortcuts.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="284">
   <si>
     <t>Smart code completion</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Ctrl + Alt + Shift + S</t>
   </si>
   <si>
-    <t>Reference fixed</t>
-  </si>
-  <si>
     <t>Debugging</t>
   </si>
   <si>
@@ -514,9 +511,6 @@
     <t>Move Line Up/Down</t>
   </si>
   <si>
-    <t>Reference added</t>
-  </si>
-  <si>
     <t>Undo/Redo</t>
   </si>
   <si>
@@ -679,9 +673,6 @@
     <t>Ctrl + Alt + Z</t>
   </si>
   <si>
-    <t>Shortcut fixed</t>
-  </si>
-  <si>
     <t>Ctrl + Alt + F12</t>
   </si>
   <si>
@@ -872,6 +863,12 @@
   </si>
   <si>
     <t>Extend / Shrink selection</t>
+  </si>
+  <si>
+    <t>Maven Projects</t>
+  </si>
+  <si>
+    <t>Alt + Shift + Q, B</t>
   </si>
 </sst>
 </file>
@@ -895,7 +892,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -914,26 +911,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -961,109 +940,35 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1372,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,18 +1294,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="D1" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="25"/>
-      <c r="G1" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" s="25"/>
+      <c r="B1" s="13"/>
+      <c r="D1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="G1" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1410,24 +1315,24 @@
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>199</v>
+      <c r="A3" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>283</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>0</v>
@@ -1436,38 +1341,38 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>229</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>197</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>2</v>
@@ -1476,84 +1381,84 @@
         <v>3</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+    <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>185</v>
+      <c r="E9" s="12" t="s">
+        <v>183</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>5</v>
@@ -1563,117 +1468,117 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="B11" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="H11" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="5" t="s">
+      <c r="D13" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="G14" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="D13" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="D14" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="H14" s="3" t="s">
+    <row r="15" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="D15" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1681,19 +1586,19 @@
         <v>156</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>162</v>
+        <v>151</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1701,673 +1606,673 @@
         <v>155</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H17" s="3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="D20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="15"/>
-      <c r="D19" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="H20" s="27" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>195</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>272</v>
+        <v>30</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>273</v>
+        <v>31</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>195</v>
+        <v>269</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>196</v>
+        <v>270</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>247</v>
+        <v>193</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>246</v>
+        <v>194</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="B27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="H26" s="3" t="s">
+      <c r="G27" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="D27" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" s="3" t="s">
+    <row r="28" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="D28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="H27" s="3" t="s">
+      <c r="G28" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="D29" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="16"/>
-      <c r="D28" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>94</v>
+        <v>205</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="B31" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="G31" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>283</v>
+      <c r="D32" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>91</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>167</v>
+        <v>211</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>90</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>173</v>
+        <v>52</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>89</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>228</v>
+        <v>81</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>88</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>257</v>
+        <v>82</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>87</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="G38" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="H38" s="25"/>
+      <c r="D38" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>171</v>
+      <c r="D39" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H39" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G40" s="7" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="D40" s="8" t="s">
+      <c r="H40" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E40" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="H40" s="12" t="s">
+      <c r="E41" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="H41" s="3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D41" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="H41" s="3" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B43" s="9"/>
+      <c r="D43" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="H43" s="8" t="s">
         <v>264</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="B42" s="15"/>
-      <c r="D42" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="G43" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="H43" s="12" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>161</v>
+        <v>214</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D44" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+      <c r="B46" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="E46" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D46" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="G46" s="15" t="s">
+      <c r="G46" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H46" s="9"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="16"/>
+      <c r="B50" s="16"/>
+      <c r="D50" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H46" s="15"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D49" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="G49" s="2" t="s">
+      <c r="H50" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="16"/>
+      <c r="B51" s="16"/>
+      <c r="D51" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="H49" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+      <c r="H51" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B50" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" s="20" t="s">
-        <v>260</v>
-      </c>
-      <c r="D51" s="11" t="s">
+      <c r="B52" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E51" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="B52" s="22"/>
-      <c r="D52" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="H52" s="12" t="s">
-        <v>252</v>
+      <c r="G52" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Intellij Shortcuts & Code Coverage
</commit_message>
<xml_diff>
--- a/IntelliJ-Shortcuts.xlsx
+++ b/IntelliJ-Shortcuts.xlsx
@@ -34,9 +34,6 @@
     <t>Ctrl + P</t>
   </si>
   <si>
-    <t>Recent files popup</t>
-  </si>
-  <si>
     <t>Ctrl + E</t>
   </si>
   <si>
@@ -857,6 +854,9 @@
   </si>
   <si>
     <t>Alt + W / Ctrl + Alt + W</t>
+  </si>
+  <si>
+    <t>Recent files &amp; Views popup</t>
   </si>
 </sst>
 </file>
@@ -1273,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A28" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,44 +1291,44 @@
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="13"/>
       <c r="D1" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="13"/>
       <c r="G1" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>248</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>249</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>0</v>
@@ -1337,38 +1337,38 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>2</v>
@@ -1377,886 +1377,886 @@
         <v>3</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="D13" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="D14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B15" s="6"/>
       <c r="D15" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>188</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="9"/>
       <c r="D20" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G20" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="D23" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>236</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>171</v>
-      </c>
       <c r="D25" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="G27" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="D28" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="G28" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="10"/>
       <c r="D29" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G29" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="D30" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="D32" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>262</v>
-      </c>
       <c r="G32" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G34" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G35" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H35" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D36" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="E36" s="8" t="s">
-        <v>279</v>
-      </c>
       <c r="G36" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D37" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D42" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G42" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="H42" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B43" s="9"/>
       <c r="D43" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="G43" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G44" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H44" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D45" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G47" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G48" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="H48" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="D49" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G49" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="H49" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="16"/>
       <c r="B50" s="16"/>
       <c r="D50" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G50" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H50" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="16"/>
       <c r="B51" s="16"/>
       <c r="G51" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G52" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="H52" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>